<commit_message>
Added payment tool column
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/payment_registry.xlsx
+++ b/src/main/resources/templates/payment_registry.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/inalarsanukaev/git/reporter/src/main/resources/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99530F67-A5F0-0E45-9B82-42B5393E5E61}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9E6CC1C-D2E2-2243-8BA7-54C695B4707A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Лист1" sheetId="2" r:id="rId1"/>
+    <sheet name="Лист2" sheetId="3" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -23,10 +23,9 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Inal Arsanukaev</author>
-    <author/>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{5F3A2B74-2DBF-414B-A424-2177C9DFC74B}">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{AD6C514F-EBAE-D047-A833-B90F2082CDA1}">
       <text>
         <r>
           <rPr>
@@ -60,20 +59,82 @@
         </r>
       </text>
     </comment>
-    <comment ref="A3" authorId="1" shapeId="0" xr:uid="{E3949544-2CE4-E84D-B10E-5CC08CF349A4}">
+    <comment ref="A3" authorId="0" shapeId="0" xr:uid="{BC6D339C-2806-2B42-85E5-653E88422C2C}">
       <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t>Inal Arsanukaev:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
         <r>
           <rPr>
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Helvetica Neue"/>
           </rPr>
-          <t>jx:each(items="payments" var="payment" lastCell="H3")</t>
+          <t>jx:each(items="payments" var="payment" lastCell="H3</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Helvetica Neue"/>
+          </rPr>
+          <t>"</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t>)</t>
         </r>
       </text>
     </comment>
-    <comment ref="A9" authorId="1" shapeId="0" xr:uid="{8FCB8013-E956-4346-801F-DC644935F9ED}">
+    <comment ref="A9" authorId="0" shapeId="0" xr:uid="{B2634855-EC06-5C4D-ACBA-5D71F5868DA5}">
       <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t>Inal Arsanukaev:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
         <r>
           <rPr>
             <sz val="10"/>
@@ -81,6 +142,15 @@
             <rFont val="Helvetica Neue"/>
           </rPr>
           <t>jx:each(items="refunds" var="refund" lastCell="H9")</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Helvetica Neue"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
         </r>
       </text>
     </comment>
@@ -100,9 +170,6 @@
     <t>Id платежа</t>
   </si>
   <si>
-    <t>Карта</t>
-  </si>
-  <si>
     <t>Сумма платежа</t>
   </si>
   <si>
@@ -124,9 +191,6 @@
     <t>${payment.id}</t>
   </si>
   <si>
-    <t>${payment.cardNum}</t>
-  </si>
-  <si>
     <t>${payment.amount}</t>
   </si>
   <si>
@@ -175,9 +239,6 @@
     <t>${refund.amount}</t>
   </si>
   <si>
-    <t>${refund.cardNum}</t>
-  </si>
-  <si>
     <t>${refund.payerEmail}</t>
   </si>
   <si>
@@ -188,6 +249,15 @@
   </si>
   <si>
     <t>${totalRefundAmnt}</t>
+  </si>
+  <si>
+    <t>Метод оплаты</t>
+  </si>
+  <si>
+    <t>${payment.paymentTool}</t>
+  </si>
+  <si>
+    <t>${refund.paymentTool}</t>
   </si>
 </sst>
 </file>
@@ -498,7 +568,7 @@
         <xdr:cNvPr id="2" name="AutoShape 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{67E3023A-1921-9B4E-80A2-B608C62D0227}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{67D03413-87E5-494B-8B61-D70BDEC36C4F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -552,7 +622,7 @@
         <xdr:cNvPr id="3" name="AutoShape 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{324D08E0-3661-AE4C-B40F-958E45E222B8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9D217645-B287-604B-BF7C-EB72A78BBAD3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -606,7 +676,7 @@
         <xdr:cNvPr id="4" name="AutoShape 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A5F032E8-B091-6D4E-ACAA-2CEEB19A7482}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4C0E85E7-F399-3D49-8259-6224895A3B62}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -660,7 +730,7 @@
         <xdr:cNvPr id="5" name="AutoShape 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BC61AB7D-F495-2241-8C2E-8DB81A865C38}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{36ACD439-3B18-8946-A290-DB97D51AF1D7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -995,11 +1065,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87E2301A-B294-BB4C-A750-49108B988711}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF46ABAF-F9CC-B046-AD3D-15C16BFEABBD}">
   <dimension ref="A1:J999"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:H1"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1038,65 +1108,65 @@
         <v>2</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="F2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="G2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>7</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>8</v>
       </c>
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
     </row>
     <row r="3" spans="1:10" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="C3" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="E3" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="F3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="G3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="H3" s="4" t="s">
         <v>14</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>16</v>
       </c>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
     </row>
     <row r="4" spans="1:10" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A4" s="17" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B4" s="18"/>
       <c r="C4" s="19"/>
       <c r="D4" s="11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F4" s="5"/>
       <c r="G4" s="8"/>
@@ -1130,7 +1200,7 @@
     </row>
     <row r="7" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="14" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B7" s="15"/>
       <c r="C7" s="15"/>
@@ -1144,68 +1214,68 @@
     </row>
     <row r="8" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>2</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="F8" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G8" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="G8" s="7" t="s">
+      <c r="H8" s="7" t="s">
         <v>7</v>
-      </c>
-      <c r="H8" s="7" t="s">
-        <v>8</v>
       </c>
       <c r="I8" s="8"/>
       <c r="J8" s="8"/>
     </row>
     <row r="9" spans="1:10" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="D9" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="E9" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F9" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="D9" s="13" t="s">
+      <c r="G9" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E9" s="8" t="s">
+      <c r="H9" s="8" t="s">
         <v>28</v>
-      </c>
-      <c r="F9" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="G9" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="H9" s="8" t="s">
-        <v>31</v>
       </c>
       <c r="I9" s="8"/>
       <c r="J9" s="8"/>
     </row>
     <row r="10" spans="1:10" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A10" s="17" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B10" s="18"/>
       <c r="C10" s="19"/>
       <c r="D10" s="11" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E10" s="5"/>
       <c r="F10" s="8"/>
@@ -2332,6 +2402,7 @@
     <mergeCell ref="A10:C10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>

</xml_diff>